<commit_message>
Update heterogeneity analysis output with confidence intervals
</commit_message>
<xml_diff>
--- a/Tables/t2_ITT.xlsx
+++ b/Tables/t2_ITT.xlsx
@@ -21,10 +21,19 @@
     <t>Outcome</t>
   </si>
   <si>
+    <t>Male condom attitudes index</t>
+  </si>
+  <si>
     <t>Used male condom at most recent sex (0/1)</t>
   </si>
   <si>
-    <t>Male condom attitudes index</t>
+    <t>Contraceptive knowledge index</t>
+  </si>
+  <si>
+    <t>Modern contraceptive methods known (n)</t>
+  </si>
+  <si>
+    <t>Discussed contraceptive use with recent partner (0/1)</t>
   </si>
   <si>
     <t>Can identify a female condom (0/1)</t>
@@ -45,22 +54,22 @@
     <t>Used a female condom at most recent sex (0/1)</t>
   </si>
   <si>
-    <t>Contraceptive knowledge index</t>
-  </si>
-  <si>
-    <t>Modern contraceptive methods known (n)</t>
-  </si>
-  <si>
-    <t>Discussed contraceptive use with recent partner (0/1)</t>
-  </si>
-  <si>
     <t>Control</t>
   </si>
   <si>
+    <t>0.07 (1.03)</t>
+  </si>
+  <si>
     <t>528 (43.07%)</t>
   </si>
   <si>
-    <t>0.07 (1.03)</t>
+    <t>0.34 (0.98)</t>
+  </si>
+  <si>
+    <t>5.87 (2.52)</t>
+  </si>
+  <si>
+    <t>890 (72.89%)</t>
   </si>
   <si>
     <t>678 (55.30%)</t>
@@ -81,22 +90,22 @@
     <t>8 (0.65%)</t>
   </si>
   <si>
-    <t>0.34 (0.98)</t>
-  </si>
-  <si>
-    <t>5.87 (2.52)</t>
-  </si>
-  <si>
-    <t>890 (72.89%)</t>
-  </si>
-  <si>
     <t>Treatment</t>
   </si>
   <si>
+    <t>0.04 (0.97)</t>
+  </si>
+  <si>
     <t>540 (44.85%)</t>
   </si>
   <si>
-    <t>0.04 (0.97)</t>
+    <t>0.37 (0.94)</t>
+  </si>
+  <si>
+    <t>5.84 (2.58)</t>
+  </si>
+  <si>
+    <t>881 (73.72%)</t>
   </si>
   <si>
     <t>724 (60.13%)</t>
@@ -117,25 +126,25 @@
     <t>9 (0.75%)</t>
   </si>
   <si>
-    <t>0.37 (0.94)</t>
-  </si>
-  <si>
-    <t>5.84 (2.58)</t>
-  </si>
-  <si>
-    <t>881 (73.72%)</t>
-  </si>
-  <si>
     <t>Crude</t>
   </si>
   <si>
     <t>RD</t>
   </si>
   <si>
+    <t xml:space="preserve">   -0.031</t>
+  </si>
+  <si>
     <t xml:space="preserve">    0.018</t>
   </si>
   <si>
-    <t xml:space="preserve">   -0.031</t>
+    <t xml:space="preserve">    0.029</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -0.033</t>
+  </si>
+  <si>
+    <t xml:space="preserve">    0.008</t>
   </si>
   <si>
     <t xml:space="preserve">    0.048</t>
@@ -153,22 +162,22 @@
     <t xml:space="preserve">    0.001</t>
   </si>
   <si>
-    <t xml:space="preserve">    0.029</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -0.033</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    0.008</t>
-  </si>
-  <si>
     <t>95% CI</t>
   </si>
   <si>
+    <t>(-0.167, 0.106)</t>
+  </si>
+  <si>
     <t>(-0.065, 0.101)</t>
   </si>
   <si>
-    <t>(-0.167, 0.106)</t>
+    <t>(-0.090, 0.148)</t>
+  </si>
+  <si>
+    <t>(-0.332, 0.265)</t>
+  </si>
+  <si>
+    <t>(-0.056, 0.072)</t>
   </si>
   <si>
     <t>(-0.014, 0.111)</t>
@@ -189,21 +198,15 @@
     <t>(-0.006, 0.008)</t>
   </si>
   <si>
-    <t>(-0.090, 0.148)</t>
-  </si>
-  <si>
-    <t>(-0.332, 0.265)</t>
-  </si>
-  <si>
-    <t>(-0.056, 0.072)</t>
-  </si>
-  <si>
     <t>OR</t>
   </si>
   <si>
     <t xml:space="preserve">     1.08</t>
   </si>
   <si>
+    <t xml:space="preserve">     1.04</t>
+  </si>
+  <si>
     <t xml:space="preserve">     1.22</t>
   </si>
   <si>
@@ -219,12 +222,12 @@
     <t xml:space="preserve">     1.15</t>
   </si>
   <si>
-    <t xml:space="preserve">     1.04</t>
-  </si>
-  <si>
     <t>(0.77, 1.50)</t>
   </si>
   <si>
+    <t>(0.75, 1.45)</t>
+  </si>
+  <si>
     <t>(0.94, 1.57)</t>
   </si>
   <si>
@@ -240,15 +243,18 @@
     <t>(0.43, 3.09)</t>
   </si>
   <si>
-    <t>(0.75, 1.45)</t>
-  </si>
-  <si>
     <t>Adjusted</t>
   </si>
   <si>
     <t xml:space="preserve">   -0.002</t>
   </si>
   <si>
+    <t xml:space="preserve">   -0.020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   -0.012</t>
+  </si>
+  <si>
     <t xml:space="preserve">    0.048+</t>
   </si>
   <si>
@@ -264,16 +270,19 @@
     <t xml:space="preserve">    0.007</t>
   </si>
   <si>
-    <t xml:space="preserve">   -0.020</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   -0.012</t>
+    <t>(-0.103, 0.125)</t>
   </si>
   <si>
     <t>(-0.046, 0.041)</t>
   </si>
   <si>
-    <t>(-0.103, 0.125)</t>
+    <t>(-0.068, 0.125)</t>
+  </si>
+  <si>
+    <t>(-0.327, 0.287)</t>
+  </si>
+  <si>
+    <t>(-0.065, 0.040)</t>
   </si>
   <si>
     <t>(0.001, 0.096)</t>
@@ -291,18 +300,12 @@
     <t>(-0.003, 0.012)</t>
   </si>
   <si>
-    <t>(-0.068, 0.125)</t>
-  </si>
-  <si>
-    <t>(-0.327, 0.287)</t>
-  </si>
-  <si>
-    <t>(-0.065, 0.040)</t>
-  </si>
-  <si>
     <t xml:space="preserve">     0.98</t>
   </si>
   <si>
+    <t xml:space="preserve">     0.94</t>
+  </si>
+  <si>
     <t xml:space="preserve">     1.23*</t>
   </si>
   <si>
@@ -312,12 +315,12 @@
     <t xml:space="preserve">     2.02</t>
   </si>
   <si>
-    <t xml:space="preserve">     0.94</t>
-  </si>
-  <si>
     <t>(0.77, 1.23)</t>
   </si>
   <si>
+    <t>(0.72, 1.24)</t>
+  </si>
+  <si>
     <t>(1.00, 1.52)</t>
   </si>
   <si>
@@ -331,9 +334,6 @@
   </si>
   <si>
     <t>(0.66, 6.22)</t>
-  </si>
-  <si>
-    <t>(0.72, 1.24)</t>
   </si>
 </sst>
 </file>
@@ -467,22 +467,22 @@
         <v>50</v>
       </c>
       <c r="F3" t="s">
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>69</v>
+        <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="I3" t="s">
         <v>85</v>
       </c>
       <c r="J3" t="s">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>100</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -502,22 +502,22 @@
         <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>0</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="H4" t="s">
-        <v>42</v>
+        <v>77</v>
       </c>
       <c r="I4" t="s">
         <v>86</v>
       </c>
       <c r="J4" t="s">
-        <v>0</v>
+        <v>95</v>
       </c>
       <c r="K4" t="s">
-        <v>0</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5">
@@ -537,22 +537,22 @@
         <v>52</v>
       </c>
       <c r="F5" t="s">
-        <v>63</v>
+        <v>0</v>
       </c>
       <c r="G5" t="s">
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>78</v>
+        <v>41</v>
       </c>
       <c r="I5" t="s">
         <v>87</v>
       </c>
       <c r="J5" t="s">
-        <v>96</v>
+        <v>0</v>
       </c>
       <c r="K5" t="s">
-        <v>101</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -572,22 +572,22 @@
         <v>53</v>
       </c>
       <c r="F6" t="s">
-        <v>64</v>
+        <v>0</v>
       </c>
       <c r="G6" t="s">
-        <v>71</v>
+        <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I6" t="s">
         <v>88</v>
       </c>
       <c r="J6" t="s">
-        <v>95</v>
+        <v>0</v>
       </c>
       <c r="K6" t="s">
-        <v>102</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -601,28 +601,28 @@
         <v>30</v>
       </c>
       <c r="D7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="E7" t="s">
         <v>54</v>
       </c>
       <c r="F7" t="s">
-        <v>0</v>
+        <v>63</v>
       </c>
       <c r="G7" t="s">
-        <v>0</v>
+        <v>70</v>
       </c>
       <c r="H7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I7" t="s">
         <v>89</v>
       </c>
       <c r="J7" t="s">
-        <v>0</v>
+        <v>96</v>
       </c>
       <c r="K7" t="s">
-        <v>0</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8">
@@ -636,28 +636,28 @@
         <v>31</v>
       </c>
       <c r="D8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E8" t="s">
         <v>55</v>
       </c>
       <c r="F8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>90</v>
       </c>
       <c r="J8" t="s">
-        <v>65</v>
+        <v>97</v>
       </c>
       <c r="K8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="9">
@@ -671,28 +671,28 @@
         <v>32</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
         <v>56</v>
       </c>
       <c r="F9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G9" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I9" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="J9" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="10">
@@ -706,28 +706,28 @@
         <v>33</v>
       </c>
       <c r="D10" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="E10" t="s">
         <v>57</v>
       </c>
       <c r="F10" t="s">
-        <v>67</v>
+        <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>74</v>
+        <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>44</v>
+        <v>82</v>
       </c>
       <c r="I10" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="J10" t="s">
-        <v>98</v>
+        <v>0</v>
       </c>
       <c r="K10" t="s">
-        <v>105</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -747,22 +747,22 @@
         <v>58</v>
       </c>
       <c r="F11" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="G11" t="s">
-        <v>0</v>
+        <v>73</v>
       </c>
       <c r="H11" t="s">
-        <v>46</v>
+        <v>83</v>
       </c>
       <c r="I11" t="s">
-        <v>92</v>
+        <v>58</v>
       </c>
       <c r="J11" t="s">
-        <v>0</v>
+        <v>66</v>
       </c>
       <c r="K11" t="s">
-        <v>0</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12">
@@ -782,22 +782,22 @@
         <v>59</v>
       </c>
       <c r="F12" t="s">
-        <v>0</v>
+        <v>67</v>
       </c>
       <c r="G12" t="s">
-        <v>0</v>
+        <v>74</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="I12" t="s">
         <v>93</v>
       </c>
       <c r="J12" t="s">
-        <v>0</v>
+        <v>98</v>
       </c>
       <c r="K12" t="s">
-        <v>0</v>
+        <v>105</v>
       </c>
     </row>
     <row r="13">
@@ -823,7 +823,7 @@
         <v>75</v>
       </c>
       <c r="H13" t="s">
-        <v>84</v>
+        <v>47</v>
       </c>
       <c r="I13" t="s">
         <v>94</v>

</xml_diff>